<commit_message>
Updating code and dataout files
</commit_message>
<xml_diff>
--- a/dataIn/resultsmanPergusa.xlsx
+++ b/dataIn/resultsmanPergusa.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Scripts\stsRankBuilder\dataIn\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -2658,9 +2663,6 @@
     <t>77</t>
   </si>
   <si>
-    <t>DAVí</t>
-  </si>
-  <si>
     <t>DANIELE</t>
   </si>
   <si>
@@ -2893,6 +2895,9 @@
   </si>
   <si>
     <t>00:33:57</t>
+  </si>
+  <si>
+    <t>DAVI</t>
   </si>
 </sst>
 </file>
@@ -2936,6 +2941,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3263,26 +3276,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="15" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="15" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3332,7 +3345,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3382,7 +3395,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3432,7 +3445,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3482,7 +3495,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3532,7 +3545,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3582,7 +3595,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3632,7 +3645,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3682,7 +3695,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3732,7 +3745,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3779,7 +3792,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3829,7 +3842,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3876,7 +3889,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3926,7 +3939,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3973,7 +3986,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4020,7 +4033,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4070,7 +4083,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4117,7 +4130,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4164,7 +4177,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4211,7 +4224,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4255,7 +4268,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4302,7 +4315,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4352,7 +4365,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4399,7 +4412,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4449,7 +4462,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4496,7 +4509,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4546,7 +4559,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4593,7 +4606,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4640,7 +4653,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4687,7 +4700,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4737,7 +4750,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4784,7 +4797,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4831,7 +4844,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4881,7 +4894,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4928,7 +4941,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4978,7 +4991,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -5028,7 +5041,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5078,7 +5091,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5125,7 +5138,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5172,7 +5185,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5222,7 +5235,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5272,7 +5285,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5319,7 +5332,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5366,7 +5379,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5416,7 +5429,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5466,7 +5479,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5513,7 +5526,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5560,7 +5573,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5610,7 +5623,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5657,7 +5670,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5704,7 +5717,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -5754,7 +5767,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -5804,7 +5817,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -5851,7 +5864,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5901,7 +5914,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -5951,7 +5964,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -6001,7 +6014,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -6048,7 +6061,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -6095,7 +6108,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -6142,7 +6155,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -6186,7 +6199,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -6236,7 +6249,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -6286,7 +6299,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -6336,7 +6349,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -6386,7 +6399,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -6436,7 +6449,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -6483,7 +6496,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -6533,7 +6546,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -6583,7 +6596,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="69" spans="1:16">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -6633,7 +6646,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="70" spans="1:16">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -6680,7 +6693,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -6730,7 +6743,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -6780,7 +6793,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -6830,7 +6843,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -6880,7 +6893,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -6927,7 +6940,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="76" spans="1:16">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -6977,7 +6990,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="77" spans="1:16">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -7024,7 +7037,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -7074,7 +7087,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="79" spans="1:16">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -7124,7 +7137,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -7174,7 +7187,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="81" spans="1:16">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -7221,7 +7234,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="82" spans="1:16">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -7271,7 +7284,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="83" spans="1:16">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -7318,7 +7331,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="84" spans="1:16">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -7368,7 +7381,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="85" spans="1:16">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -7415,7 +7428,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="86" spans="1:16">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -7465,7 +7478,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="87" spans="1:16">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -7515,7 +7528,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="88" spans="1:16">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -7562,7 +7575,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="89" spans="1:16">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -7609,7 +7622,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="90" spans="1:16">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -7656,7 +7669,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="91" spans="1:16">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -7706,7 +7719,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="92" spans="1:16">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -7756,7 +7769,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="93" spans="1:16">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -7806,7 +7819,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="94" spans="1:16">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -7853,7 +7866,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="95" spans="1:16">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -7900,7 +7913,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="96" spans="1:16">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -7950,7 +7963,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="97" spans="1:16">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -7997,7 +8010,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="98" spans="1:16">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -8047,7 +8060,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="99" spans="1:16">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -8055,10 +8068,10 @@
         <v>878</v>
       </c>
       <c r="C99" t="s">
+        <v>957</v>
+      </c>
+      <c r="D99" t="s">
         <v>879</v>
-      </c>
-      <c r="D99" t="s">
-        <v>880</v>
       </c>
       <c r="E99" t="s">
         <v>19</v>
@@ -8073,10 +8086,10 @@
         <v>83</v>
       </c>
       <c r="I99" t="s">
+        <v>880</v>
+      </c>
+      <c r="J99" t="s">
         <v>881</v>
-      </c>
-      <c r="J99" t="s">
-        <v>882</v>
       </c>
       <c r="K99" t="s">
         <v>539</v>
@@ -8085,27 +8098,27 @@
         <v>583</v>
       </c>
       <c r="M99" t="s">
+        <v>882</v>
+      </c>
+      <c r="N99" t="s">
         <v>883</v>
       </c>
-      <c r="N99" t="s">
+      <c r="O99" t="s">
         <v>884</v>
       </c>
-      <c r="O99" t="s">
+      <c r="P99" t="s">
         <v>885</v>
       </c>
-      <c r="P99" t="s">
-        <v>886</v>
-      </c>
-    </row>
-    <row r="100" spans="1:16">
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
       <c r="B100" t="s">
+        <v>886</v>
+      </c>
+      <c r="C100" t="s">
         <v>887</v>
-      </c>
-      <c r="C100" t="s">
-        <v>888</v>
       </c>
       <c r="D100" t="s">
         <v>537</v>
@@ -8114,48 +8127,48 @@
         <v>19</v>
       </c>
       <c r="F100" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="G100" t="s">
         <v>16</v>
       </c>
       <c r="H100" t="s">
+        <v>889</v>
+      </c>
+      <c r="I100" t="s">
         <v>890</v>
       </c>
-      <c r="I100" t="s">
+      <c r="J100" t="s">
         <v>891</v>
       </c>
-      <c r="J100" t="s">
+      <c r="K100" t="s">
         <v>892</v>
-      </c>
-      <c r="K100" t="s">
-        <v>893</v>
       </c>
       <c r="L100" t="s">
         <v>737</v>
       </c>
       <c r="M100" t="s">
+        <v>893</v>
+      </c>
+      <c r="N100" t="s">
         <v>894</v>
       </c>
-      <c r="N100" t="s">
+      <c r="O100" t="s">
         <v>895</v>
       </c>
-      <c r="O100" t="s">
+      <c r="P100" t="s">
         <v>896</v>
       </c>
-      <c r="P100" t="s">
-        <v>897</v>
-      </c>
-    </row>
-    <row r="101" spans="1:16">
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
       <c r="B101" t="s">
+        <v>897</v>
+      </c>
+      <c r="C101" t="s">
         <v>898</v>
-      </c>
-      <c r="C101" t="s">
-        <v>899</v>
       </c>
       <c r="D101" t="s">
         <v>537</v>
@@ -8173,39 +8186,39 @@
         <v>360</v>
       </c>
       <c r="I101" t="s">
+        <v>899</v>
+      </c>
+      <c r="J101" t="s">
         <v>900</v>
       </c>
-      <c r="J101" t="s">
+      <c r="K101" t="s">
         <v>901</v>
-      </c>
-      <c r="K101" t="s">
-        <v>902</v>
       </c>
       <c r="L101" t="s">
         <v>208</v>
       </c>
       <c r="M101" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="N101" t="s">
         <v>265</v>
       </c>
       <c r="O101" t="s">
+        <v>903</v>
+      </c>
+      <c r="P101" t="s">
         <v>904</v>
       </c>
-      <c r="P101" t="s">
-        <v>905</v>
-      </c>
-    </row>
-    <row r="102" spans="1:16">
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
       <c r="B102" t="s">
+        <v>905</v>
+      </c>
+      <c r="C102" t="s">
         <v>906</v>
-      </c>
-      <c r="C102" t="s">
-        <v>907</v>
       </c>
       <c r="D102" t="s">
         <v>32</v>
@@ -8223,36 +8236,36 @@
         <v>360</v>
       </c>
       <c r="I102" t="s">
+        <v>907</v>
+      </c>
+      <c r="K102" t="s">
         <v>908</v>
-      </c>
-      <c r="K102" t="s">
-        <v>909</v>
       </c>
       <c r="L102" t="s">
         <v>239</v>
       </c>
       <c r="M102" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="N102" t="s">
         <v>397</v>
       </c>
       <c r="O102" t="s">
+        <v>910</v>
+      </c>
+      <c r="P102" t="s">
         <v>911</v>
       </c>
-      <c r="P102" t="s">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="103" spans="1:16">
+    </row>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
       <c r="B103" t="s">
+        <v>912</v>
+      </c>
+      <c r="C103" t="s">
         <v>913</v>
-      </c>
-      <c r="C103" t="s">
-        <v>914</v>
       </c>
       <c r="D103" t="s">
         <v>537</v>
@@ -8270,28 +8283,28 @@
         <v>70</v>
       </c>
       <c r="I103" t="s">
+        <v>914</v>
+      </c>
+      <c r="K103" t="s">
         <v>915</v>
-      </c>
-      <c r="K103" t="s">
-        <v>916</v>
       </c>
       <c r="L103" t="s">
         <v>172</v>
       </c>
       <c r="M103" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="N103" t="s">
         <v>755</v>
       </c>
       <c r="O103" t="s">
+        <v>917</v>
+      </c>
+      <c r="P103" t="s">
         <v>918</v>
       </c>
-      <c r="P103" t="s">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="104" spans="1:16">
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -8299,10 +8312,10 @@
         <v>860</v>
       </c>
       <c r="C104" t="s">
+        <v>919</v>
+      </c>
+      <c r="D104" t="s">
         <v>920</v>
-      </c>
-      <c r="D104" t="s">
-        <v>921</v>
       </c>
       <c r="E104" t="s">
         <v>19</v>
@@ -8317,36 +8330,36 @@
         <v>21</v>
       </c>
       <c r="I104" t="s">
+        <v>921</v>
+      </c>
+      <c r="K104" t="s">
         <v>922</v>
-      </c>
-      <c r="K104" t="s">
-        <v>923</v>
       </c>
       <c r="L104" t="s">
         <v>203</v>
       </c>
       <c r="M104" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="N104" t="s">
         <v>241</v>
       </c>
       <c r="O104" t="s">
+        <v>924</v>
+      </c>
+      <c r="P104" t="s">
         <v>925</v>
       </c>
-      <c r="P104" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="105" spans="1:16">
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
       <c r="B105" t="s">
+        <v>926</v>
+      </c>
+      <c r="C105" t="s">
         <v>927</v>
-      </c>
-      <c r="C105" t="s">
-        <v>928</v>
       </c>
       <c r="D105" t="s">
         <v>285</v>
@@ -8355,7 +8368,7 @@
         <v>19</v>
       </c>
       <c r="F105" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="G105" t="s">
         <v>741</v>
@@ -8364,10 +8377,10 @@
         <v>70</v>
       </c>
       <c r="I105" t="s">
+        <v>929</v>
+      </c>
+      <c r="J105" t="s">
         <v>930</v>
-      </c>
-      <c r="J105" t="s">
-        <v>931</v>
       </c>
       <c r="K105" t="s">
         <v>515</v>
@@ -8376,36 +8389,36 @@
         <v>230</v>
       </c>
       <c r="M105" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="N105" t="s">
         <v>469</v>
       </c>
       <c r="O105" t="s">
+        <v>932</v>
+      </c>
+      <c r="P105" t="s">
         <v>933</v>
       </c>
-      <c r="P105" t="s">
-        <v>934</v>
-      </c>
-    </row>
-    <row r="106" spans="1:16">
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
       <c r="B106" t="s">
+        <v>934</v>
+      </c>
+      <c r="C106" t="s">
         <v>935</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D106" t="s">
         <v>936</v>
       </c>
-      <c r="D106" t="s">
+      <c r="E106" t="s">
+        <v>19</v>
+      </c>
+      <c r="F106" t="s">
         <v>937</v>
-      </c>
-      <c r="E106" t="s">
-        <v>19</v>
-      </c>
-      <c r="F106" t="s">
-        <v>938</v>
       </c>
       <c r="G106" t="s">
         <v>283</v>
@@ -8414,16 +8427,16 @@
         <v>34</v>
       </c>
       <c r="I106" t="s">
+        <v>938</v>
+      </c>
+      <c r="K106" t="s">
         <v>939</v>
-      </c>
-      <c r="K106" t="s">
-        <v>940</v>
       </c>
       <c r="L106" t="s">
         <v>652</v>
       </c>
       <c r="M106" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="N106" t="s">
         <v>334</v>
@@ -8432,18 +8445,18 @@
         <v>423</v>
       </c>
       <c r="P106" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>942</v>
       </c>
-    </row>
-    <row r="107" spans="1:16">
-      <c r="A107" t="s">
+      <c r="B107" t="s">
         <v>943</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
         <v>944</v>
-      </c>
-      <c r="C107" t="s">
-        <v>945</v>
       </c>
       <c r="D107" t="s">
         <v>45</v>
@@ -8455,30 +8468,30 @@
         <v>501</v>
       </c>
       <c r="G107" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="H107" t="s">
         <v>34</v>
       </c>
       <c r="I107" t="s">
+        <v>945</v>
+      </c>
+      <c r="K107" t="s">
         <v>946</v>
-      </c>
-      <c r="K107" t="s">
-        <v>947</v>
       </c>
       <c r="L107" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="108" spans="1:16">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B108" t="s">
+        <v>947</v>
+      </c>
+      <c r="C108" t="s">
         <v>948</v>
-      </c>
-      <c r="C108" t="s">
-        <v>949</v>
       </c>
       <c r="D108" t="s">
         <v>537</v>
@@ -8490,33 +8503,33 @@
         <v>69</v>
       </c>
       <c r="G108" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="H108" t="s">
         <v>70</v>
       </c>
       <c r="I108" t="s">
+        <v>949</v>
+      </c>
+      <c r="K108" t="s">
         <v>950</v>
-      </c>
-      <c r="K108" t="s">
-        <v>951</v>
       </c>
       <c r="L108" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="109" spans="1:16">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B109" t="s">
+        <v>951</v>
+      </c>
+      <c r="C109" t="s">
         <v>952</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D109" t="s">
         <v>953</v>
-      </c>
-      <c r="D109" t="s">
-        <v>954</v>
       </c>
       <c r="E109" t="s">
         <v>19</v>
@@ -8525,22 +8538,22 @@
         <v>157</v>
       </c>
       <c r="G109" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="H109" t="s">
         <v>70</v>
       </c>
       <c r="I109" t="s">
+        <v>954</v>
+      </c>
+      <c r="K109" t="s">
         <v>955</v>
-      </c>
-      <c r="K109" t="s">
-        <v>956</v>
       </c>
       <c r="L109" t="s">
         <v>241</v>
       </c>
       <c r="M109" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
   </sheetData>

</xml_diff>